<commit_message>
analysed the heart disease dataset
</commit_message>
<xml_diff>
--- a/diabetes_analysis.xlsx
+++ b/diabetes_analysis.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhD CamTue\Projects\SSL with cause and effect features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{028A137C-2618-460C-BCA4-1C21CB509750}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC9D746-1466-4028-BBC6-C82F38B106BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="diabetes" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -561,7 +561,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -578,6 +578,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -933,11 +936,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I769"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23252,11 +23255,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23315,7 +23318,7 @@
       <c r="D2" s="3">
         <v>2.5090974224840198E-21</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="7">
         <v>1.1072070213249E-2</v>
       </c>
       <c r="F2" s="2">

</xml_diff>